<commit_message>
built out stylized home page and dell page
</commit_message>
<xml_diff>
--- a/Quote Import Template.xlsx
+++ b/Quote Import Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wwt-my.sharepoint.com/personal/diestelw_wwt_com/Documents/Scripts/OrcaTweek/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wwt-my.sharepoint.com/personal/diestelw_wwt_com/Documents/Scripts/OrcaTweak/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{EC8F14E7-F53A-480F-8FBE-820F2A857A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{290866D6-DAC9-472E-8DFE-88211945D98F}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{EC8F14E7-F53A-480F-8FBE-820F2A857A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72D0ACA2-7B64-4083-B7D3-AAB375EC20BB}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -446,22 +446,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>